<commit_message>
feat: separando em backend e frontend
</commit_message>
<xml_diff>
--- a/data/arquivo_excel.xlsx
+++ b/data/arquivo_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\Projeto-I\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{488572F8-5480-430D-89A3-E9E1BC364A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F720FED-2B5D-49E1-9C6C-8231C50CCB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{72903207-C70C-45F2-8212-6FAF3885DBEB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -94,69 +94,6 @@
   </si>
   <si>
     <t>valor</t>
-  </si>
-  <si>
-    <t>produto</t>
-  </si>
-  <si>
-    <t>Produto A</t>
-  </si>
-  <si>
-    <t>Produto B</t>
-  </si>
-  <si>
-    <t>Produto C</t>
-  </si>
-  <si>
-    <t>Produto D</t>
-  </si>
-  <si>
-    <t>Produto E</t>
-  </si>
-  <si>
-    <t>Produto F</t>
-  </si>
-  <si>
-    <t>Produto G</t>
-  </si>
-  <si>
-    <t>Produto H</t>
-  </si>
-  <si>
-    <t>Produto I</t>
-  </si>
-  <si>
-    <t>Produto J</t>
-  </si>
-  <si>
-    <t>Produto K</t>
-  </si>
-  <si>
-    <t>Produto L</t>
-  </si>
-  <si>
-    <t>Produto M</t>
-  </si>
-  <si>
-    <t>Produto N</t>
-  </si>
-  <si>
-    <t>Produto O</t>
-  </si>
-  <si>
-    <t>Produto P</t>
-  </si>
-  <si>
-    <t>Produto Q</t>
-  </si>
-  <si>
-    <t>Produto R</t>
-  </si>
-  <si>
-    <t>Produto S</t>
-  </si>
-  <si>
-    <t>Produto T</t>
   </si>
   <si>
     <t>quantidade</t>
@@ -179,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -218,7 +155,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B745C3-FAA9-4624-B4BF-3CE79BD5A51B}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +484,7 @@
     <col min="3" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,13 +498,10 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -577,17 +511,14 @@
       <c r="C2" s="2">
         <v>150.5</v>
       </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -597,17 +528,14 @@
       <c r="C3" s="2">
         <v>200</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -617,17 +545,14 @@
       <c r="C4" s="2">
         <v>350.75</v>
       </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -637,17 +562,14 @@
       <c r="C5" s="2">
         <v>99.99</v>
       </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -657,17 +579,14 @@
       <c r="C6" s="2">
         <v>499.99</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -677,17 +596,14 @@
       <c r="C7" s="2">
         <v>249</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -697,17 +613,14 @@
       <c r="C8" s="2">
         <v>300</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -717,17 +630,14 @@
       <c r="C9" s="2">
         <v>450.5</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -737,17 +647,14 @@
       <c r="C10" s="2">
         <v>129.94999999999999</v>
       </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10">
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -757,17 +664,14 @@
       <c r="C11" s="2">
         <v>89.9</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -777,17 +681,14 @@
       <c r="C12" s="2">
         <v>199.9</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12">
+      <c r="D12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -797,17 +698,14 @@
       <c r="C13" s="2">
         <v>149.5</v>
       </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13">
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -817,17 +715,14 @@
       <c r="C14" s="2">
         <v>229</v>
       </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14">
+      <c r="D14">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -837,17 +732,14 @@
       <c r="C15" s="2">
         <v>309.99</v>
       </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15">
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -857,17 +749,14 @@
       <c r="C16" s="2">
         <v>299</v>
       </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16">
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -877,17 +766,14 @@
       <c r="C17" s="2">
         <v>129</v>
       </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17">
+      <c r="D17">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -897,17 +783,14 @@
       <c r="C18" s="2">
         <v>159.99</v>
       </c>
-      <c r="D18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18">
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -917,17 +800,14 @@
       <c r="C19" s="2">
         <v>289.95</v>
       </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19">
+      <c r="D19">
         <v>3</v>
       </c>
-      <c r="F19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -937,17 +817,14 @@
       <c r="C20" s="2">
         <v>349.9</v>
       </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20">
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -957,14 +834,11 @@
       <c r="C21" s="2">
         <v>399.99</v>
       </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>47</v>
+      <c r="E21" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>